<commit_message>
Refactored all test cases
</commit_message>
<xml_diff>
--- a/tendercuts/app/inventory/tests/test.xlsx
+++ b/tendercuts/app/inventory/tests/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="38400" yWindow="0" windowWidth="19200" windowHeight="21080"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Dispath sheet" sheetId="6" r:id="rId1"/>
@@ -429,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -579,15 +579,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -623,7 +614,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -764,9 +755,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1102,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="E5" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1114,23 +1102,22 @@
     <col min="2" max="2" width="43.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" customWidth="1"/>
-    <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" customWidth="1"/>
-    <col min="10" max="10" width="19.1640625" customWidth="1"/>
-    <col min="11" max="11" width="7.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" style="1" customWidth="1"/>
-    <col min="16" max="17" width="17.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.5" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="17.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:18" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
@@ -1150,9 +1137,8 @@
       <c r="O1" s="49"/>
       <c r="P1" s="49"/>
       <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="50" t="s">
         <v>59</v>
       </c>
@@ -1172,9 +1158,8 @@
       <c r="O2" s="50"/>
       <c r="P2" s="50"/>
       <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="49" t="s">
         <v>67</v>
       </c>
@@ -1194,35 +1179,33 @@
       <c r="O3" s="49"/>
       <c r="P3" s="49"/>
       <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-    </row>
-    <row r="4" spans="1:19" ht="22" thickTop="1" thickBot="1">
+    </row>
+    <row r="4" spans="1:18" ht="22" thickTop="1" thickBot="1">
       <c r="A4" s="51" t="s">
         <v>71</v>
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
       <c r="D4" s="51"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="46" t="s">
+      <c r="E4" s="46" t="s">
         <v>64</v>
       </c>
+      <c r="F4" s="47"/>
       <c r="G4" s="47"/>
       <c r="H4" s="47"/>
       <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="43" t="s">
+      <c r="J4" s="48"/>
+      <c r="K4" s="43" t="s">
         <v>65</v>
       </c>
+      <c r="L4" s="44"/>
       <c r="M4" s="44"/>
       <c r="N4" s="44"/>
       <c r="O4" s="44"/>
       <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="45"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="Q4" s="45"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="39" t="s">
         <v>72</v>
       </c>
@@ -1235,48 +1218,47 @@
       <c r="D5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="37" t="s">
+        <v>73</v>
+      </c>
       <c r="F5" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="L5" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="M5" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="N5" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="O5" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="P5" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="M5" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="O5" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="P5" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q5" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="R5" s="36" t="s">
+      <c r="Q5" s="36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="21" customHeight="1">
+    <row r="6" spans="1:18" ht="21" customHeight="1">
       <c r="A6" s="42">
         <v>319</v>
       </c>
@@ -1289,33 +1271,33 @@
       <c r="D6" s="13">
         <v>500</v>
       </c>
-      <c r="E6" s="13">
-        <v>14</v>
+      <c r="E6" s="14">
+        <v>5</v>
       </c>
       <c r="F6" s="14">
+        <v>6</v>
+      </c>
+      <c r="G6" s="14">
+        <v>2</v>
+      </c>
+      <c r="H6" s="14">
+        <v>2</v>
+      </c>
+      <c r="I6" s="14">
         <v>5</v>
       </c>
-      <c r="G6" s="14">
-        <v>6</v>
-      </c>
-      <c r="H6" s="14">
-        <v>2</v>
-      </c>
-      <c r="I6" s="14">
-        <v>2</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14">
         <v>5</v>
       </c>
-      <c r="K6" s="14"/>
       <c r="L6" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M6" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6" s="14">
         <v>2</v>
@@ -1323,16 +1305,13 @@
       <c r="P6" s="14">
         <v>2</v>
       </c>
-      <c r="Q6" s="14">
-        <v>2</v>
-      </c>
-      <c r="R6" s="8">
-        <f>L6+M6+N6+O6+P6</f>
+      <c r="Q6" s="8">
+        <f>K6+L6+M6+N6+O6</f>
         <v>12</v>
       </c>
-      <c r="S6" s="30"/>
-    </row>
-    <row r="7" spans="1:19" ht="21" customHeight="1">
+      <c r="R6" s="30"/>
+    </row>
+    <row r="7" spans="1:18" ht="21" customHeight="1">
       <c r="A7" s="42">
         <v>195</v>
       </c>
@@ -1345,48 +1324,45 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="13">
-        <v>30</v>
+      <c r="E7" s="14">
+        <v>18</v>
       </c>
       <c r="F7" s="14">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G7" s="14">
+        <v>2</v>
+      </c>
+      <c r="H7" s="14">
+        <v>2</v>
+      </c>
+      <c r="I7" s="14">
         <v>8</v>
       </c>
-      <c r="H7" s="14">
-        <v>2</v>
-      </c>
-      <c r="I7" s="14">
-        <v>2</v>
-      </c>
-      <c r="J7" s="14">
-        <v>8</v>
-      </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14">
-        <v>1</v>
-      </c>
-      <c r="M7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14">
+        <v>1</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14">
+        <v>2</v>
+      </c>
       <c r="N7" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O7" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P7" s="14">
         <v>3</v>
       </c>
-      <c r="Q7" s="14">
-        <v>3</v>
-      </c>
-      <c r="R7" s="8">
-        <f t="shared" ref="R7:R18" si="0">L7+M7+N7+O7+P7</f>
+      <c r="Q7" s="8">
+        <f t="shared" ref="Q7:Q18" si="0">K7+L7+M7+N7+O7</f>
         <v>10</v>
       </c>
-      <c r="S7" s="30"/>
-    </row>
-    <row r="8" spans="1:19" ht="21" customHeight="1">
+      <c r="R7" s="30"/>
+    </row>
+    <row r="8" spans="1:18" ht="21" customHeight="1">
       <c r="A8" s="42">
         <v>192</v>
       </c>
@@ -1399,46 +1375,43 @@
       <c r="D8" s="13">
         <v>500</v>
       </c>
-      <c r="E8" s="13">
-        <v>9</v>
+      <c r="E8" s="14">
+        <v>99</v>
       </c>
       <c r="F8" s="14">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G8" s="14">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H8" s="14">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I8" s="14">
-        <v>96</v>
-      </c>
-      <c r="J8" s="14">
         <v>95</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14">
         <v>4</v>
       </c>
+      <c r="L8" s="14"/>
       <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
+      <c r="N8" s="14">
+        <v>1</v>
+      </c>
       <c r="O8" s="14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P8" s="14">
         <v>6</v>
       </c>
-      <c r="Q8" s="14">
-        <v>6</v>
-      </c>
-      <c r="R8" s="8">
+      <c r="Q8" s="8">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="S8" s="30"/>
-    </row>
-    <row r="9" spans="1:19" ht="21" customHeight="1">
+      <c r="R8" s="30"/>
+    </row>
+    <row r="9" spans="1:18" ht="21" customHeight="1">
       <c r="A9" s="42">
         <v>193</v>
       </c>
@@ -1451,50 +1424,47 @@
       <c r="D9" s="13">
         <v>500</v>
       </c>
-      <c r="E9" s="13">
-        <v>100</v>
+      <c r="E9" s="14">
+        <v>37</v>
       </c>
       <c r="F9" s="14">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="G9" s="14">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="H9" s="14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I9" s="14">
-        <v>8</v>
-      </c>
-      <c r="J9" s="14">
         <v>45</v>
       </c>
-      <c r="K9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14">
+        <v>21</v>
+      </c>
       <c r="L9" s="14">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="M9" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N9" s="14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O9" s="14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P9" s="14">
         <v>3</v>
       </c>
-      <c r="Q9" s="14">
-        <v>3</v>
-      </c>
-      <c r="R9" s="8">
+      <c r="Q9" s="8">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="S9" s="30"/>
-    </row>
-    <row r="10" spans="1:19" ht="21" customHeight="1">
+      <c r="R9" s="30"/>
+    </row>
+    <row r="10" spans="1:18" ht="21" customHeight="1">
       <c r="A10" s="42">
         <v>197</v>
       </c>
@@ -1507,25 +1477,25 @@
       <c r="D10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="13">
-        <v>10</v>
+      <c r="E10" s="14">
+        <v>4</v>
       </c>
       <c r="F10" s="14">
         <v>4</v>
       </c>
       <c r="G10" s="14">
+        <v>0</v>
+      </c>
+      <c r="H10" s="14">
         <v>4</v>
       </c>
-      <c r="H10" s="14">
-        <v>0</v>
-      </c>
       <c r="I10" s="14">
-        <v>4</v>
-      </c>
-      <c r="J10" s="14">
-        <v>2</v>
-      </c>
-      <c r="K10" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14">
+        <v>2</v>
+      </c>
       <c r="L10" s="14">
         <v>2</v>
       </c>
@@ -1533,24 +1503,21 @@
         <v>2</v>
       </c>
       <c r="N10" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O10" s="14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P10" s="14">
         <v>5</v>
       </c>
-      <c r="Q10" s="14">
-        <v>5</v>
-      </c>
-      <c r="R10" s="8">
+      <c r="Q10" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="S10" s="30"/>
-    </row>
-    <row r="11" spans="1:19" ht="21" customHeight="1">
+      <c r="R10" s="30"/>
+    </row>
+    <row r="11" spans="1:18" ht="21" customHeight="1">
       <c r="A11" s="42">
         <v>198</v>
       </c>
@@ -1563,50 +1530,47 @@
       <c r="D11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="13">
-        <v>6</v>
+      <c r="E11" s="14">
+        <v>2</v>
       </c>
       <c r="F11" s="14">
         <v>2</v>
       </c>
       <c r="G11" s="14">
-        <v>2</v>
-      </c>
-      <c r="H11" s="14">
-        <v>1</v>
-      </c>
-      <c r="I11" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="14">
-        <v>2</v>
-      </c>
-      <c r="K11" s="14"/>
+      <c r="I11" s="14">
+        <v>2</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14">
+        <v>5</v>
+      </c>
       <c r="L11" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M11" s="14">
-        <v>3</v>
-      </c>
-      <c r="N11" s="14">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="N11" s="38" t="s">
+        <v>69</v>
       </c>
       <c r="O11" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P11" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="Q11" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="R11" s="8">
+      <c r="Q11" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="S11" s="30"/>
-    </row>
-    <row r="12" spans="1:19" ht="21" customHeight="1">
+      <c r="R11" s="30"/>
+    </row>
+    <row r="12" spans="1:18" ht="21" customHeight="1">
       <c r="A12" s="42">
         <v>199</v>
       </c>
@@ -1619,42 +1583,39 @@
       <c r="D12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="13">
-        <v>50</v>
+      <c r="E12" s="14">
+        <v>27</v>
       </c>
       <c r="F12" s="14">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="G12" s="14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H12" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12" s="14">
-        <v>4</v>
-      </c>
-      <c r="J12" s="14">
         <v>17</v>
       </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14">
+      <c r="J12" s="14"/>
+      <c r="K12" s="14">
         <v>5</v>
       </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14">
-        <v>2</v>
-      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14">
+        <v>2</v>
+      </c>
+      <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="8">
+      <c r="Q12" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="S12" s="30"/>
-    </row>
-    <row r="13" spans="1:19" ht="21" customHeight="1">
+      <c r="R12" s="30"/>
+    </row>
+    <row r="13" spans="1:18" ht="21" customHeight="1">
       <c r="A13" s="42">
         <v>196</v>
       </c>
@@ -1667,44 +1628,41 @@
       <c r="D13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="13">
-        <v>8</v>
-      </c>
-      <c r="F13" s="14">
+      <c r="E13" s="14">
         <v>5</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14">
+        <v>0</v>
+      </c>
       <c r="H13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="14">
-        <v>1</v>
-      </c>
-      <c r="J13" s="14">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
+      <c r="M13" s="14">
+        <v>2</v>
+      </c>
       <c r="N13" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="14">
         <v>2</v>
       </c>
-      <c r="Q13" s="14">
-        <v>2</v>
-      </c>
-      <c r="R13" s="8">
+      <c r="Q13" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="S13" s="30"/>
-    </row>
-    <row r="14" spans="1:19" ht="21" customHeight="1">
+      <c r="R13" s="30"/>
+    </row>
+    <row r="14" spans="1:18" ht="21" customHeight="1">
       <c r="A14" s="42">
         <v>300</v>
       </c>
@@ -1717,44 +1675,41 @@
       <c r="D14" s="13">
         <v>500</v>
       </c>
-      <c r="E14" s="13">
-        <v>15</v>
+      <c r="E14" s="14">
+        <v>6</v>
       </c>
       <c r="F14" s="14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G14" s="14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H14" s="14">
         <v>2</v>
       </c>
       <c r="I14" s="14">
-        <v>2</v>
-      </c>
-      <c r="J14" s="14">
         <v>5</v>
       </c>
+      <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
+      <c r="N14" s="14">
+        <v>1</v>
+      </c>
       <c r="O14" s="14">
         <v>1</v>
       </c>
       <c r="P14" s="14">
         <v>1</v>
       </c>
-      <c r="Q14" s="14">
-        <v>1</v>
-      </c>
-      <c r="R14" s="8">
+      <c r="Q14" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="S14" s="30"/>
-    </row>
-    <row r="15" spans="1:19" ht="21" customHeight="1">
+      <c r="R14" s="30"/>
+    </row>
+    <row r="15" spans="1:18" ht="21" customHeight="1">
       <c r="A15" s="42">
         <v>235</v>
       </c>
@@ -1767,38 +1722,35 @@
       <c r="D15" s="13">
         <v>1</v>
       </c>
-      <c r="E15" s="13">
-        <v>4</v>
-      </c>
+      <c r="E15" s="14"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="14">
+        <v>2</v>
+      </c>
       <c r="H15" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" s="14">
         <v>1</v>
       </c>
-      <c r="J15" s="14">
-        <v>1</v>
-      </c>
-      <c r="K15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14">
+        <v>2</v>
+      </c>
       <c r="L15" s="14">
-        <v>2</v>
-      </c>
-      <c r="M15" s="14">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="8">
+      <c r="Q15" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="S15" s="30"/>
-    </row>
-    <row r="16" spans="1:19" ht="21" customHeight="1">
+      <c r="R15" s="30"/>
+    </row>
+    <row r="16" spans="1:18" ht="21" customHeight="1">
       <c r="A16" s="42">
         <v>236</v>
       </c>
@@ -1811,42 +1763,39 @@
       <c r="D16" s="13">
         <v>1</v>
       </c>
-      <c r="E16" s="13">
-        <v>7</v>
+      <c r="E16" s="14">
+        <v>1</v>
       </c>
       <c r="F16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="14">
         <v>1</v>
       </c>
       <c r="I16" s="14">
-        <v>1</v>
-      </c>
-      <c r="J16" s="14">
-        <v>2</v>
-      </c>
-      <c r="K16" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14">
+        <v>1</v>
+      </c>
       <c r="L16" s="14">
         <v>1</v>
       </c>
-      <c r="M16" s="14">
-        <v>1</v>
-      </c>
+      <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
       <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="8">
+      <c r="Q16" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="S16" s="30"/>
-    </row>
-    <row r="17" spans="1:19" ht="21" customHeight="1">
+      <c r="R16" s="30"/>
+    </row>
+    <row r="17" spans="1:18" ht="21" customHeight="1">
       <c r="A17" s="42">
         <v>200</v>
       </c>
@@ -1859,11 +1808,11 @@
       <c r="D17" s="13">
         <v>500</v>
       </c>
-      <c r="E17" s="13">
-        <v>6</v>
+      <c r="E17" s="14">
+        <v>2</v>
       </c>
       <c r="F17" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="14">
         <v>1</v>
@@ -1872,35 +1821,32 @@
         <v>1</v>
       </c>
       <c r="I17" s="14">
-        <v>1</v>
-      </c>
-      <c r="J17" s="14">
-        <v>2</v>
-      </c>
-      <c r="K17" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14">
+        <v>1</v>
+      </c>
       <c r="L17" s="14">
         <v>1</v>
       </c>
-      <c r="M17" s="14">
-        <v>1</v>
-      </c>
-      <c r="N17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14">
+        <v>1</v>
+      </c>
       <c r="O17" s="14">
         <v>1</v>
       </c>
       <c r="P17" s="14">
         <v>1</v>
       </c>
-      <c r="Q17" s="14">
-        <v>1</v>
-      </c>
-      <c r="R17" s="8">
+      <c r="Q17" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="S17" s="30"/>
-    </row>
-    <row r="18" spans="1:19" ht="21" customHeight="1">
+      <c r="R17" s="30"/>
+    </row>
+    <row r="18" spans="1:18" ht="21" customHeight="1">
       <c r="A18" s="42">
         <v>329</v>
       </c>
@@ -1913,14 +1859,14 @@
       <c r="D18" s="13">
         <v>500</v>
       </c>
-      <c r="E18" s="13">
-        <v>4</v>
+      <c r="E18" s="14">
+        <v>1</v>
       </c>
       <c r="F18" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="14">
         <v>1</v>
@@ -1928,95 +1874,90 @@
       <c r="I18" s="14">
         <v>1</v>
       </c>
-      <c r="J18" s="14">
-        <v>1</v>
-      </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14">
-        <v>1</v>
-      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14">
+        <v>1</v>
+      </c>
+      <c r="L18" s="14"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
       <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="8">
+      <c r="Q18" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="S18" s="30"/>
-    </row>
-    <row r="19" spans="1:19">
+      <c r="R18" s="30"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="B19" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="30"/>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="R19" s="30"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="B20" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="37" t="s">
+        <v>73</v>
+      </c>
       <c r="F20" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="L20" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="37" t="s">
+      <c r="M20" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="I20" s="37" t="s">
+      <c r="N20" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J20" s="37" t="s">
+      <c r="O20" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="K20" s="37" t="s">
+      <c r="P20" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L20" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="M20" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="N20" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="O20" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="P20" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q20" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="R20" s="7" t="s">
+      <c r="Q20" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="S20" s="30"/>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="R20" s="30"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="42">
         <v>307</v>
       </c>
@@ -2029,30 +1970,30 @@
       <c r="D21" s="13">
         <v>500</v>
       </c>
-      <c r="E21" s="13">
-        <v>7</v>
+      <c r="E21" s="14">
+        <v>2</v>
       </c>
       <c r="F21" s="14">
         <v>2</v>
       </c>
       <c r="G21" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="14">
         <v>1</v>
       </c>
       <c r="I21" s="14">
-        <v>1</v>
-      </c>
-      <c r="J21" s="14">
-        <v>3</v>
-      </c>
-      <c r="K21" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14">
+        <v>4</v>
+      </c>
       <c r="L21" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M21" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N21" s="14">
         <v>1</v>
@@ -2063,16 +2004,13 @@
       <c r="P21" s="14">
         <v>1</v>
       </c>
-      <c r="Q21" s="14">
-        <v>1</v>
-      </c>
-      <c r="R21" s="8">
-        <f t="shared" ref="R21:R29" si="1">L21+M21+N21+O21+P21</f>
+      <c r="Q21" s="8">
+        <f t="shared" ref="Q21:Q29" si="1">K21+L21+M21+N21+O21</f>
         <v>9</v>
       </c>
-      <c r="S21" s="30"/>
-    </row>
-    <row r="22" spans="1:19" ht="18.75" customHeight="1">
+      <c r="R21" s="30"/>
+    </row>
+    <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="42">
         <v>308</v>
       </c>
@@ -2085,48 +2023,45 @@
       <c r="D22" s="13">
         <v>250</v>
       </c>
-      <c r="E22" s="13">
-        <v>11</v>
+      <c r="E22" s="14">
+        <v>5</v>
       </c>
       <c r="F22" s="14">
+        <v>8</v>
+      </c>
+      <c r="G22" s="14">
+        <v>0</v>
+      </c>
+      <c r="H22" s="14">
+        <v>2</v>
+      </c>
+      <c r="I22" s="14">
+        <v>4</v>
+      </c>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14">
         <v>5</v>
       </c>
-      <c r="G22" s="14">
-        <v>8</v>
-      </c>
-      <c r="H22" s="14">
-        <v>0</v>
-      </c>
-      <c r="I22" s="14">
-        <v>2</v>
-      </c>
-      <c r="J22" s="14">
-        <v>4</v>
-      </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14">
+      <c r="L22" s="14"/>
+      <c r="M22" s="14">
+        <v>2</v>
+      </c>
+      <c r="N22" s="14">
+        <v>1</v>
+      </c>
+      <c r="O22" s="14">
         <v>5</v>
-      </c>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14">
-        <v>2</v>
-      </c>
-      <c r="O22" s="14">
-        <v>1</v>
       </c>
       <c r="P22" s="14">
         <v>5</v>
       </c>
-      <c r="Q22" s="14">
-        <v>5</v>
-      </c>
-      <c r="R22" s="8">
+      <c r="Q22" s="8">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="S22" s="30"/>
-    </row>
-    <row r="23" spans="1:19" ht="18.75" customHeight="1">
+      <c r="R22" s="30"/>
+    </row>
+    <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="42">
         <v>306</v>
       </c>
@@ -2139,46 +2074,43 @@
       <c r="D23" s="13">
         <v>300</v>
       </c>
-      <c r="E23" s="13">
-        <v>4</v>
+      <c r="E23" s="14">
+        <v>3</v>
       </c>
       <c r="F23" s="14">
         <v>3</v>
       </c>
       <c r="G23" s="14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H23" s="14">
         <v>0</v>
       </c>
       <c r="I23" s="14">
-        <v>0</v>
-      </c>
-      <c r="J23" s="14">
-        <v>1</v>
-      </c>
-      <c r="K23" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14">
+        <v>3</v>
+      </c>
       <c r="L23" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M23" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N23" s="14">
         <v>1</v>
       </c>
-      <c r="O23" s="14">
-        <v>1</v>
-      </c>
+      <c r="O23" s="14"/>
       <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="8">
+      <c r="Q23" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="S23" s="30"/>
-    </row>
-    <row r="24" spans="1:19" ht="21.75" customHeight="1">
+      <c r="R23" s="30"/>
+    </row>
+    <row r="24" spans="1:18" ht="21.75" customHeight="1">
       <c r="A24" s="42">
         <v>304</v>
       </c>
@@ -2191,48 +2123,45 @@
       <c r="D24" s="13">
         <v>500</v>
       </c>
-      <c r="E24" s="13">
-        <v>22</v>
+      <c r="E24" s="14">
+        <v>8</v>
       </c>
       <c r="F24" s="14">
+        <v>10</v>
+      </c>
+      <c r="G24" s="14">
+        <v>3</v>
+      </c>
+      <c r="H24" s="14">
+        <v>3</v>
+      </c>
+      <c r="I24" s="14">
         <v>8</v>
       </c>
-      <c r="G24" s="14">
-        <v>10</v>
-      </c>
-      <c r="H24" s="14">
-        <v>3</v>
-      </c>
-      <c r="I24" s="14">
-        <v>3</v>
-      </c>
-      <c r="J24" s="14">
-        <v>8</v>
-      </c>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14">
+      <c r="J24" s="14"/>
+      <c r="K24" s="14">
         <v>5</v>
       </c>
-      <c r="M24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14">
+        <v>1</v>
+      </c>
       <c r="N24" s="14">
         <v>1</v>
       </c>
       <c r="O24" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P24" s="14">
         <v>3</v>
       </c>
-      <c r="Q24" s="14">
-        <v>3</v>
-      </c>
-      <c r="R24" s="8">
+      <c r="Q24" s="8">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="S24" s="30"/>
-    </row>
-    <row r="25" spans="1:19">
+      <c r="R24" s="30"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="42">
         <v>305</v>
       </c>
@@ -2245,48 +2174,45 @@
       <c r="D25" s="13">
         <v>250</v>
       </c>
-      <c r="E25" s="13">
-        <v>8</v>
+      <c r="E25" s="14">
+        <v>5</v>
       </c>
       <c r="F25" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G25" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H25" s="14">
         <v>0</v>
       </c>
       <c r="I25" s="14">
-        <v>0</v>
-      </c>
-      <c r="J25" s="14">
-        <v>3</v>
-      </c>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14">
-        <v>1</v>
-      </c>
-      <c r="M25" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14">
+        <v>1</v>
+      </c>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14">
+        <v>2</v>
+      </c>
       <c r="N25" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O25" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P25" s="14">
         <v>2</v>
       </c>
-      <c r="Q25" s="14">
-        <v>2</v>
-      </c>
-      <c r="R25" s="8">
+      <c r="Q25" s="8">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="S25" s="30"/>
-    </row>
-    <row r="26" spans="1:19">
+      <c r="R25" s="30"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="42">
         <v>309</v>
       </c>
@@ -2299,14 +2225,14 @@
       <c r="D26" s="13">
         <v>500</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="14">
         <v>2</v>
       </c>
       <c r="F26" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="14">
         <v>0</v>
@@ -2314,27 +2240,24 @@
       <c r="I26" s="14">
         <v>0</v>
       </c>
-      <c r="J26" s="14">
-        <v>0</v>
-      </c>
-      <c r="K26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14">
+        <v>2</v>
+      </c>
       <c r="L26" s="14">
         <v>2</v>
       </c>
-      <c r="M26" s="14">
-        <v>2</v>
-      </c>
+      <c r="M26" s="14"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="8">
+      <c r="Q26" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="S26" s="30"/>
-    </row>
-    <row r="27" spans="1:19">
+      <c r="R26" s="30"/>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="42">
         <v>303</v>
       </c>
@@ -2347,14 +2270,14 @@
       <c r="D27" s="13">
         <v>500</v>
       </c>
-      <c r="E27" s="13">
-        <v>10</v>
+      <c r="E27" s="14">
+        <v>4</v>
       </c>
       <c r="F27" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G27" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27" s="14">
         <v>2</v>
@@ -2362,29 +2285,26 @@
       <c r="I27" s="14">
         <v>2</v>
       </c>
-      <c r="J27" s="14">
-        <v>2</v>
-      </c>
+      <c r="J27" s="14"/>
       <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14">
-        <v>6</v>
-      </c>
+      <c r="L27" s="14">
+        <v>6</v>
+      </c>
+      <c r="M27" s="14"/>
       <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
+      <c r="O27" s="14">
+        <v>1</v>
+      </c>
       <c r="P27" s="14">
         <v>1</v>
       </c>
-      <c r="Q27" s="14">
-        <v>1</v>
-      </c>
-      <c r="R27" s="8">
+      <c r="Q27" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="S27" s="30"/>
-    </row>
-    <row r="28" spans="1:19">
+      <c r="R27" s="30"/>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="42">
         <v>298</v>
       </c>
@@ -2397,19 +2317,19 @@
       <c r="D28" s="13">
         <v>500</v>
       </c>
-      <c r="E28" s="13">
-        <v>2</v>
-      </c>
-      <c r="F28" s="14">
-        <v>1</v>
-      </c>
+      <c r="E28" s="14">
+        <v>1</v>
+      </c>
+      <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14">
-        <v>1</v>
-      </c>
-      <c r="K28" s="14"/>
+      <c r="I28" s="14">
+        <v>1</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14">
+        <v>1</v>
+      </c>
       <c r="L28" s="14">
         <v>1</v>
       </c>
@@ -2425,16 +2345,13 @@
       <c r="P28" s="14">
         <v>1</v>
       </c>
-      <c r="Q28" s="14">
-        <v>1</v>
-      </c>
-      <c r="R28" s="8">
+      <c r="Q28" s="8">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="S28" s="30"/>
-    </row>
-    <row r="29" spans="1:19">
+      <c r="R28" s="30"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="42">
         <v>299</v>
       </c>
@@ -2447,68 +2364,64 @@
       <c r="D29" s="13">
         <v>500</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="14">
+        <v>1</v>
+      </c>
+      <c r="F29" s="14">
+        <v>1</v>
+      </c>
+      <c r="G29" s="14">
+        <v>1</v>
+      </c>
+      <c r="H29" s="14">
+        <v>2</v>
+      </c>
+      <c r="I29" s="14">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14">
+        <v>2</v>
+      </c>
+      <c r="L29" s="14">
+        <v>2</v>
+      </c>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14">
         <v>4</v>
       </c>
-      <c r="F29" s="14">
-        <v>1</v>
-      </c>
-      <c r="G29" s="14">
-        <v>1</v>
-      </c>
-      <c r="H29" s="14">
-        <v>1</v>
-      </c>
-      <c r="I29" s="14">
-        <v>2</v>
-      </c>
-      <c r="J29" s="14">
-        <v>0</v>
-      </c>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14">
-        <v>2</v>
-      </c>
-      <c r="M29" s="14">
-        <v>2</v>
-      </c>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
       <c r="P29" s="14">
         <v>4</v>
       </c>
-      <c r="Q29" s="14">
-        <v>4</v>
-      </c>
-      <c r="R29" s="8">
+      <c r="Q29" s="8">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="S29" s="30"/>
-    </row>
-    <row r="30" spans="1:19">
+      <c r="R29" s="30"/>
+    </row>
+    <row r="30" spans="1:18">
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="31"/>
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="31"/>
       <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
+      <c r="K30" s="32"/>
       <c r="L30" s="32"/>
       <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
-      <c r="O30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="9"/>
       <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="30"/>
-    </row>
-    <row r="31" spans="1:19">
+      <c r="Q30" s="3"/>
+      <c r="R30" s="30"/>
+    </row>
+    <row r="31" spans="1:18">
       <c r="B31" s="11" t="s">
         <v>1</v>
       </c>
@@ -2518,49 +2431,48 @@
       <c r="D31" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="11"/>
+      <c r="E31" s="37" t="s">
+        <v>73</v>
+      </c>
       <c r="F31" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="J31" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="K31" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="L31" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="H31" s="37" t="s">
+      <c r="M31" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="I31" s="37" t="s">
+      <c r="N31" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J31" s="37" t="s">
+      <c r="O31" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="K31" s="37" t="s">
+      <c r="P31" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L31" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="M31" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="N31" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="O31" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="P31" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q31" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="R31" s="10" t="s">
+      <c r="Q31" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S31" s="30"/>
-    </row>
-    <row r="32" spans="1:19">
+      <c r="R31" s="30"/>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="42">
         <v>220</v>
       </c>
@@ -2573,50 +2485,47 @@
       <c r="D32" s="13">
         <v>500</v>
       </c>
-      <c r="E32" s="13">
-        <v>11</v>
+      <c r="E32" s="14">
+        <v>0</v>
       </c>
       <c r="F32" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G32" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H32" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32" s="14">
         <v>2</v>
       </c>
       <c r="J32" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K32" s="14">
         <v>3</v>
       </c>
       <c r="L32" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M32" s="14">
-        <v>2</v>
-      </c>
-      <c r="N32" s="14">
-        <v>1</v>
-      </c>
-      <c r="O32" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14">
+        <v>1</v>
+      </c>
       <c r="P32" s="14">
         <v>1</v>
       </c>
-      <c r="Q32" s="14">
-        <v>1</v>
-      </c>
-      <c r="R32" s="8">
-        <f t="shared" ref="R32:R38" si="2">L32+M32+N32+O32+P32</f>
+      <c r="Q32" s="8">
+        <f t="shared" ref="Q32:Q38" si="2">K32+L32+M32+N32+O32</f>
         <v>7</v>
       </c>
-      <c r="S32" s="30"/>
-    </row>
-    <row r="33" spans="1:19">
+      <c r="R32" s="30"/>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="42">
         <v>216</v>
       </c>
@@ -2629,42 +2538,39 @@
       <c r="D33" s="13">
         <v>500</v>
       </c>
-      <c r="E33" s="13">
-        <v>11</v>
+      <c r="E33" s="14">
+        <v>2</v>
       </c>
       <c r="F33" s="14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G33" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H33" s="14">
         <v>1</v>
       </c>
       <c r="I33" s="14">
-        <v>1</v>
-      </c>
-      <c r="J33" s="14">
-        <v>2</v>
-      </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14">
+        <v>1</v>
+      </c>
+      <c r="L33" s="14"/>
       <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14">
-        <v>1</v>
-      </c>
+      <c r="N33" s="14">
+        <v>1</v>
+      </c>
+      <c r="O33" s="14"/>
       <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="8">
+      <c r="Q33" s="8">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="S33" s="30"/>
-    </row>
-    <row r="34" spans="1:19">
+      <c r="R33" s="30"/>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="42">
         <v>244</v>
       </c>
@@ -2677,7 +2583,7 @@
       <c r="D34" s="13">
         <v>500</v>
       </c>
-      <c r="E34" s="13"/>
+      <c r="E34" s="14"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
@@ -2689,14 +2595,13 @@
       <c r="N34" s="14"/>
       <c r="O34" s="14"/>
       <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="8">
+      <c r="Q34" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S34" s="30"/>
-    </row>
-    <row r="35" spans="1:19">
+      <c r="R34" s="30"/>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="42">
         <v>234</v>
       </c>
@@ -2709,32 +2614,31 @@
       <c r="D35" s="13">
         <v>500</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
+      <c r="K35" s="14">
+        <v>2</v>
+      </c>
       <c r="L35" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M35" s="14">
         <v>1</v>
       </c>
-      <c r="N35" s="14">
-        <v>1</v>
-      </c>
+      <c r="N35" s="14"/>
       <c r="O35" s="14"/>
       <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="8">
+      <c r="Q35" s="8">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="S35" s="30"/>
-    </row>
-    <row r="36" spans="1:19">
+      <c r="R35" s="30"/>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="42">
         <v>245</v>
       </c>
@@ -2747,7 +2651,7 @@
       <c r="D36" s="13">
         <v>500</v>
       </c>
-      <c r="E36" s="13"/>
+      <c r="E36" s="14"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -2759,14 +2663,13 @@
       <c r="N36" s="14"/>
       <c r="O36" s="14"/>
       <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="8">
+      <c r="Q36" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S36" s="30"/>
-    </row>
-    <row r="37" spans="1:19">
+      <c r="R36" s="30"/>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37" s="42">
         <v>226</v>
       </c>
@@ -2779,48 +2682,45 @@
       <c r="D37" s="13">
         <v>500</v>
       </c>
-      <c r="E37" s="13">
-        <v>30</v>
+      <c r="E37" s="14">
+        <v>8</v>
       </c>
       <c r="F37" s="14">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G37" s="14">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H37" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I37" s="14">
-        <v>2</v>
-      </c>
-      <c r="J37" s="14">
         <v>7</v>
       </c>
-      <c r="K37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14">
+        <v>3</v>
+      </c>
       <c r="L37" s="14">
-        <v>3</v>
-      </c>
-      <c r="M37" s="14">
         <v>9</v>
       </c>
-      <c r="N37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14">
+        <v>1</v>
+      </c>
       <c r="O37" s="14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P37" s="14">
         <v>4</v>
       </c>
-      <c r="Q37" s="14">
-        <v>4</v>
-      </c>
-      <c r="R37" s="8">
+      <c r="Q37" s="8">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="S37" s="30"/>
-    </row>
-    <row r="38" spans="1:19">
+      <c r="R37" s="30"/>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="42">
         <v>218</v>
       </c>
@@ -2833,36 +2733,33 @@
       <c r="D38" s="13">
         <v>500</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="14"/>
+      <c r="F38" s="14">
         <v>4</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14">
-        <v>4</v>
-      </c>
+      <c r="G38" s="14"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
       <c r="L38" s="14"/>
       <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
+      <c r="N38" s="14">
+        <v>1</v>
+      </c>
       <c r="O38" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P38" s="14">
         <v>2</v>
       </c>
-      <c r="Q38" s="14">
-        <v>2</v>
-      </c>
-      <c r="R38" s="8">
+      <c r="Q38" s="8">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="S38" s="30"/>
-    </row>
-    <row r="39" spans="1:19">
+      <c r="R38" s="30"/>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" s="42">
         <v>317</v>
       </c>
@@ -2875,14 +2772,14 @@
       <c r="D39" s="13">
         <v>500</v>
       </c>
-      <c r="E39" s="13">
-        <v>7</v>
+      <c r="E39" s="14">
+        <v>2</v>
       </c>
       <c r="F39" s="14">
         <v>2</v>
       </c>
       <c r="G39" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" s="14">
         <v>1</v>
@@ -2890,29 +2787,26 @@
       <c r="I39" s="14">
         <v>1</v>
       </c>
-      <c r="J39" s="14">
-        <v>1</v>
-      </c>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14">
-        <v>1</v>
-      </c>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14">
+        <v>1</v>
+      </c>
+      <c r="L39" s="14"/>
       <c r="M39" s="14"/>
       <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
+      <c r="O39" s="14">
+        <v>1</v>
+      </c>
       <c r="P39" s="14">
         <v>1</v>
       </c>
-      <c r="Q39" s="14">
-        <v>1</v>
-      </c>
-      <c r="R39" s="8">
-        <f t="shared" ref="R39:R47" si="3">L39+M39+N39+O39+P39</f>
-        <v>2</v>
-      </c>
-      <c r="S39" s="30"/>
-    </row>
-    <row r="40" spans="1:19">
+      <c r="Q39" s="8">
+        <f t="shared" ref="Q39:Q47" si="3">K39+L39+M39+N39+O39</f>
+        <v>2</v>
+      </c>
+      <c r="R39" s="30"/>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="42">
         <v>222</v>
       </c>
@@ -2925,23 +2819,23 @@
       <c r="D40" s="13">
         <v>500</v>
       </c>
-      <c r="E40" s="13">
-        <v>11</v>
+      <c r="E40" s="14">
+        <v>2</v>
       </c>
       <c r="F40" s="14">
         <v>2</v>
       </c>
       <c r="G40" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H40" s="14">
         <v>1</v>
       </c>
       <c r="I40" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J40" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K40" s="14">
         <v>2</v>
@@ -2950,23 +2844,20 @@
         <v>2</v>
       </c>
       <c r="M40" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N40" s="14">
         <v>1</v>
       </c>
-      <c r="O40" s="14">
-        <v>1</v>
-      </c>
+      <c r="O40" s="14"/>
       <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="8">
+      <c r="Q40" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="S40" s="30"/>
-    </row>
-    <row r="41" spans="1:19">
+      <c r="R40" s="30"/>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" s="42">
         <v>221</v>
       </c>
@@ -2979,7 +2870,7 @@
       <c r="D41" s="13">
         <v>500</v>
       </c>
-      <c r="E41" s="13"/>
+      <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
@@ -2991,14 +2882,13 @@
       <c r="N41" s="14"/>
       <c r="O41" s="14"/>
       <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="8">
+      <c r="Q41" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S41" s="30"/>
-    </row>
-    <row r="42" spans="1:19">
+      <c r="R41" s="30"/>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="42">
         <v>246</v>
       </c>
@@ -3011,44 +2901,41 @@
       <c r="D42" s="13">
         <v>500</v>
       </c>
-      <c r="E42" s="13">
-        <v>11</v>
+      <c r="E42" s="14">
+        <v>0</v>
       </c>
       <c r="F42" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G42" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H42" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I42" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J42" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K42" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L42" s="14">
-        <v>4</v>
-      </c>
-      <c r="M42" s="14">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M42" s="14"/>
       <c r="N42" s="14"/>
       <c r="O42" s="14"/>
       <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="8">
+      <c r="Q42" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="S42" s="30"/>
-    </row>
-    <row r="43" spans="1:19">
+      <c r="R42" s="30"/>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" s="42">
         <v>217</v>
       </c>
@@ -3061,7 +2948,7 @@
       <c r="D43" s="13">
         <v>500</v>
       </c>
-      <c r="E43" s="13"/>
+      <c r="E43" s="14"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
       <c r="H43" s="14"/>
@@ -3073,14 +2960,13 @@
       <c r="N43" s="14"/>
       <c r="O43" s="14"/>
       <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="8">
+      <c r="Q43" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S43" s="30"/>
-    </row>
-    <row r="44" spans="1:19">
+      <c r="R43" s="30"/>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" s="42">
         <v>233</v>
       </c>
@@ -3093,7 +2979,7 @@
       <c r="D44" s="13">
         <v>500</v>
       </c>
-      <c r="E44" s="13"/>
+      <c r="E44" s="14"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
@@ -3105,14 +2991,13 @@
       <c r="N44" s="14"/>
       <c r="O44" s="14"/>
       <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="8">
+      <c r="Q44" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S44" s="30"/>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="R44" s="30"/>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="42">
         <v>219</v>
       </c>
@@ -3125,7 +3010,7 @@
       <c r="D45" s="13">
         <v>500</v>
       </c>
-      <c r="E45" s="13"/>
+      <c r="E45" s="14"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
@@ -3137,14 +3022,13 @@
       <c r="N45" s="14"/>
       <c r="O45" s="14"/>
       <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="8">
+      <c r="Q45" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S45" s="30"/>
-    </row>
-    <row r="46" spans="1:19">
+      <c r="R45" s="30"/>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46" s="42">
         <v>316</v>
       </c>
@@ -3155,42 +3039,39 @@
       <c r="D46" s="13">
         <v>500</v>
       </c>
-      <c r="E46" s="13">
-        <v>15</v>
+      <c r="E46" s="14">
+        <v>5</v>
       </c>
       <c r="F46" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G46" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H46" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J46" s="14">
-        <v>4</v>
-      </c>
-      <c r="K46" s="14">
-        <v>1</v>
-      </c>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14">
+        <v>6</v>
+      </c>
+      <c r="M46" s="14"/>
       <c r="N46" s="14"/>
       <c r="O46" s="14"/>
       <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="8">
+      <c r="Q46" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="S46" s="30"/>
-    </row>
-    <row r="47" spans="1:19">
+      <c r="R46" s="30"/>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47" s="42">
         <v>213</v>
       </c>
@@ -3203,56 +3084,52 @@
       <c r="D47" s="13">
         <v>500</v>
       </c>
-      <c r="E47" s="13">
-        <v>3</v>
+      <c r="E47" s="14">
+        <v>2</v>
       </c>
       <c r="F47" s="14">
-        <v>2</v>
-      </c>
-      <c r="G47" s="14">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G47" s="14"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
       <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14">
-        <v>1</v>
-      </c>
+      <c r="L47" s="14">
+        <v>1</v>
+      </c>
+      <c r="M47" s="14"/>
       <c r="N47" s="14"/>
       <c r="O47" s="14"/>
       <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="8">
+      <c r="Q47" s="8">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="S47" s="30"/>
-    </row>
-    <row r="48" spans="1:19">
+      <c r="R47" s="30"/>
+    </row>
+    <row r="48" spans="1:18">
       <c r="B48" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
+      <c r="E48" s="24"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
       <c r="H48" s="24"/>
       <c r="I48" s="24"/>
       <c r="J48" s="24"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="34"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="34"/>
+      <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
+      <c r="O48" s="5"/>
       <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="30"/>
-    </row>
-    <row r="49" spans="1:19">
+      <c r="Q48" s="6"/>
+      <c r="R48" s="30"/>
+    </row>
+    <row r="49" spans="1:18">
       <c r="B49" s="11" t="s">
         <v>1</v>
       </c>
@@ -3262,49 +3139,48 @@
       <c r="D49" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E49" s="11"/>
+      <c r="E49" s="37" t="s">
+        <v>73</v>
+      </c>
       <c r="F49" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="H49" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="I49" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="J49" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="K49" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="G49" s="37" t="s">
+      <c r="L49" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="H49" s="37" t="s">
+      <c r="M49" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="I49" s="37" t="s">
+      <c r="N49" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J49" s="37" t="s">
+      <c r="O49" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="K49" s="37" t="s">
+      <c r="P49" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L49" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="M49" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="N49" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="O49" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="P49" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q49" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="R49" s="7" t="s">
+      <c r="Q49" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="S49" s="30"/>
-    </row>
-    <row r="50" spans="1:19">
+      <c r="R49" s="30"/>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50" s="42">
         <v>237</v>
       </c>
@@ -3317,52 +3193,49 @@
       <c r="D50" s="13">
         <v>400</v>
       </c>
-      <c r="E50" s="13">
-        <v>12</v>
+      <c r="E50" s="14">
+        <v>2</v>
       </c>
       <c r="F50" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G50" s="14">
+        <v>1</v>
+      </c>
+      <c r="H50" s="14">
+        <v>1</v>
+      </c>
+      <c r="I50" s="14">
+        <v>2</v>
+      </c>
+      <c r="J50" s="14">
+        <v>2</v>
+      </c>
+      <c r="K50" s="14">
         <v>4</v>
       </c>
-      <c r="H50" s="14">
-        <v>1</v>
-      </c>
-      <c r="I50" s="14">
-        <v>1</v>
-      </c>
-      <c r="J50" s="14">
-        <v>2</v>
-      </c>
-      <c r="K50" s="14">
-        <v>2</v>
-      </c>
       <c r="L50" s="14">
+        <v>2</v>
+      </c>
+      <c r="M50" s="14">
+        <v>2</v>
+      </c>
+      <c r="N50" s="14">
+        <v>2</v>
+      </c>
+      <c r="O50" s="14">
         <v>4</v>
-      </c>
-      <c r="M50" s="14">
-        <v>2</v>
-      </c>
-      <c r="N50" s="14">
-        <v>2</v>
-      </c>
-      <c r="O50" s="14">
-        <v>2</v>
       </c>
       <c r="P50" s="14">
         <v>4</v>
       </c>
-      <c r="Q50" s="14">
-        <v>4</v>
-      </c>
-      <c r="R50" s="8">
-        <f t="shared" ref="R50:R56" si="4">L50+M50+N50+O50+P50</f>
+      <c r="Q50" s="8">
+        <f t="shared" ref="Q50:Q56" si="4">K50+L50+M50+N50+O50</f>
         <v>14</v>
       </c>
-      <c r="S50" s="30"/>
-    </row>
-    <row r="51" spans="1:19">
+      <c r="R50" s="30"/>
+    </row>
+    <row r="51" spans="1:18">
       <c r="A51" s="42">
         <v>239</v>
       </c>
@@ -3375,44 +3248,41 @@
       <c r="D51" s="13">
         <v>400</v>
       </c>
-      <c r="E51" s="13">
-        <v>3</v>
-      </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14">
-        <v>1</v>
-      </c>
-      <c r="H51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14">
+        <v>1</v>
+      </c>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14">
+        <v>1</v>
+      </c>
       <c r="I51" s="14">
         <v>1</v>
       </c>
-      <c r="J51" s="14">
-        <v>1</v>
-      </c>
-      <c r="K51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14">
+        <v>2</v>
+      </c>
       <c r="L51" s="14">
         <v>2</v>
       </c>
       <c r="M51" s="14">
-        <v>2</v>
-      </c>
-      <c r="N51" s="14">
-        <v>1</v>
-      </c>
-      <c r="O51" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14">
+        <v>1</v>
+      </c>
       <c r="P51" s="14">
         <v>1</v>
       </c>
-      <c r="Q51" s="14">
-        <v>1</v>
-      </c>
-      <c r="R51" s="8">
+      <c r="Q51" s="8">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="S51" s="30"/>
-    </row>
-    <row r="52" spans="1:19">
+      <c r="R51" s="30"/>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" s="42">
         <v>267</v>
       </c>
@@ -3425,50 +3295,47 @@
       <c r="D52" s="13">
         <v>400</v>
       </c>
-      <c r="E52" s="13">
-        <v>8</v>
+      <c r="E52" s="14">
+        <v>2</v>
       </c>
       <c r="F52" s="14">
         <v>2</v>
       </c>
       <c r="G52" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H52" s="14">
         <v>1</v>
       </c>
       <c r="I52" s="14">
-        <v>1</v>
-      </c>
-      <c r="J52" s="14">
-        <v>2</v>
-      </c>
-      <c r="K52" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14">
+        <v>1</v>
+      </c>
       <c r="L52" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M52" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N52" s="14">
         <v>1</v>
       </c>
       <c r="O52" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P52" s="14">
         <v>2</v>
       </c>
-      <c r="Q52" s="14">
-        <v>2</v>
-      </c>
-      <c r="R52" s="8">
+      <c r="Q52" s="8">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="S52" s="30"/>
-    </row>
-    <row r="53" spans="1:19">
+      <c r="R52" s="30"/>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53" s="42">
         <v>301</v>
       </c>
@@ -3481,37 +3348,34 @@
       <c r="D53" s="13">
         <v>400</v>
       </c>
-      <c r="E53" s="13">
-        <v>2</v>
-      </c>
-      <c r="F53" s="14">
-        <v>2</v>
-      </c>
+      <c r="E53" s="14">
+        <v>2</v>
+      </c>
+      <c r="F53" s="14"/>
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
       <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14">
-        <v>1</v>
-      </c>
-      <c r="N53" s="14"/>
+      <c r="L53" s="14">
+        <v>1</v>
+      </c>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14">
+        <v>1</v>
+      </c>
       <c r="O53" s="14">
         <v>1</v>
       </c>
       <c r="P53" s="14">
         <v>1</v>
       </c>
-      <c r="Q53" s="14">
-        <v>1</v>
-      </c>
-      <c r="R53" s="8">
+      <c r="Q53" s="8">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:18">
       <c r="A54" s="42">
         <v>313</v>
       </c>
@@ -3524,49 +3388,46 @@
       <c r="D54" s="13">
         <v>400</v>
       </c>
-      <c r="E54" s="13">
-        <v>8</v>
+      <c r="E54" s="14">
+        <v>1</v>
       </c>
       <c r="F54" s="14">
-        <v>1</v>
-      </c>
-      <c r="G54" s="14">
-        <v>3</v>
-      </c>
-      <c r="H54" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14">
+        <v>1</v>
+      </c>
       <c r="I54" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J54" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K54" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L54" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M54" s="14">
         <v>2</v>
       </c>
       <c r="N54" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O54" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P54" s="14">
         <v>3</v>
       </c>
-      <c r="Q54" s="14">
-        <v>3</v>
-      </c>
-      <c r="R54" s="8">
+      <c r="Q54" s="8">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:18">
       <c r="A55" s="42">
         <v>285</v>
       </c>
@@ -3579,37 +3440,36 @@
       <c r="D55" s="13">
         <v>200</v>
       </c>
-      <c r="E55" s="13"/>
+      <c r="E55" s="14"/>
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
+      <c r="K55" s="14">
+        <v>5</v>
+      </c>
       <c r="L55" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M55" s="14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N55" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O55" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P55" s="14">
         <v>4</v>
       </c>
-      <c r="Q55" s="14">
-        <v>4</v>
-      </c>
-      <c r="R55" s="8">
+      <c r="Q55" s="8">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:18">
       <c r="A56" s="42">
         <v>310</v>
       </c>
@@ -3622,51 +3482,48 @@
       <c r="D56" s="13">
         <v>400</v>
       </c>
-      <c r="E56" s="13">
-        <v>13</v>
+      <c r="E56" s="14">
+        <v>3</v>
       </c>
       <c r="F56" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G56" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H56" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56" s="14">
         <v>1</v>
       </c>
       <c r="J56" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K56" s="14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L56" s="14">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M56" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N56" s="14">
         <v>1</v>
       </c>
       <c r="O56" s="14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P56" s="14">
         <v>5</v>
       </c>
-      <c r="Q56" s="14">
-        <v>5</v>
-      </c>
-      <c r="R56" s="8">
+      <c r="Q56" s="8">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:18">
       <c r="A57" s="42">
         <v>269</v>
       </c>
@@ -3679,37 +3536,36 @@
       <c r="D57" s="13">
         <v>200</v>
       </c>
-      <c r="E57" s="13"/>
+      <c r="E57" s="14"/>
       <c r="F57" s="14"/>
       <c r="G57" s="14"/>
       <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
+      <c r="I57" s="29"/>
       <c r="J57" s="29"/>
-      <c r="K57" s="29"/>
+      <c r="K57" s="14">
+        <v>2</v>
+      </c>
       <c r="L57" s="14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M57" s="14">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N57" s="14">
         <v>1</v>
       </c>
       <c r="O57" s="14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P57" s="14">
         <v>4</v>
       </c>
-      <c r="Q57" s="14">
-        <v>4</v>
-      </c>
-      <c r="R57" s="8">
-        <f t="shared" ref="R57:R61" si="5">L57+M57+N57+O57+P57</f>
+      <c r="Q57" s="8">
+        <f t="shared" ref="Q57:Q61" si="5">K57+L57+M57+N57+O57</f>
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:18">
       <c r="A58" s="42">
         <v>302</v>
       </c>
@@ -3722,49 +3578,46 @@
       <c r="D58" s="13">
         <v>200</v>
       </c>
-      <c r="E58" s="13">
-        <v>11</v>
+      <c r="E58" s="14">
+        <v>2</v>
       </c>
       <c r="F58" s="14">
-        <v>2</v>
-      </c>
-      <c r="G58" s="14">
         <v>4</v>
       </c>
-      <c r="H58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14">
+        <v>1</v>
+      </c>
       <c r="I58" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J58" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K58" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L58" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M58" s="14">
         <v>2</v>
       </c>
       <c r="N58" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O58" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P58" s="14">
         <v>3</v>
       </c>
-      <c r="Q58" s="14">
-        <v>3</v>
-      </c>
-      <c r="R58" s="8">
+      <c r="Q58" s="8">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:18">
       <c r="A59" s="42">
         <v>241</v>
       </c>
@@ -3777,7 +3630,7 @@
       <c r="D59" s="13">
         <v>400</v>
       </c>
-      <c r="E59" s="13"/>
+      <c r="E59" s="14"/>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
@@ -3789,13 +3642,12 @@
       <c r="N59" s="14"/>
       <c r="O59" s="14"/>
       <c r="P59" s="14"/>
-      <c r="Q59" s="14"/>
-      <c r="R59" s="8">
+      <c r="Q59" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:18">
       <c r="A60" s="42">
         <v>326</v>
       </c>
@@ -3808,11 +3660,11 @@
       <c r="D60" s="13">
         <v>400</v>
       </c>
-      <c r="E60" s="13">
-        <v>5</v>
+      <c r="E60" s="14">
+        <v>2</v>
       </c>
       <c r="F60" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G60" s="14">
         <v>1</v>
@@ -3820,35 +3672,32 @@
       <c r="H60" s="14">
         <v>1</v>
       </c>
-      <c r="I60" s="14">
-        <v>1</v>
-      </c>
+      <c r="I60" s="14"/>
       <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
+      <c r="K60" s="14">
+        <v>1</v>
+      </c>
       <c r="L60" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M60" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N60" s="14">
         <v>1</v>
       </c>
       <c r="O60" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P60" s="14">
         <v>3</v>
       </c>
-      <c r="Q60" s="14">
-        <v>3</v>
-      </c>
-      <c r="R60" s="8">
+      <c r="Q60" s="8">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:18">
       <c r="A61" s="42">
         <v>331</v>
       </c>
@@ -3861,54 +3710,53 @@
       <c r="D61" s="13">
         <v>200</v>
       </c>
-      <c r="E61" s="13"/>
+      <c r="E61" s="14"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
+      <c r="K61" s="14">
+        <v>11</v>
+      </c>
       <c r="L61" s="14">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="M61" s="14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N61" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O61" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P61" s="14">
         <v>1</v>
       </c>
-      <c r="Q61" s="14">
-        <v>1</v>
-      </c>
-      <c r="R61" s="8">
+      <c r="Q61" s="8">
         <f t="shared" si="5"/>
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="20.25" customHeight="1">
+    <row r="62" spans="1:18" ht="20.25" customHeight="1">
       <c r="A62"/>
+      <c r="K62"/>
       <c r="L62"/>
       <c r="M62"/>
       <c r="N62"/>
       <c r="O62"/>
       <c r="P62"/>
       <c r="Q62"/>
-      <c r="R62"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A3:R3"/>
-    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <pageMargins left="0.16" right="0.14000000000000001" top="0.75" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="portrait"/>

</xml_diff>